<commit_message>
Flowchart Sistem Administrasi Penjualan Ancol.doc ver_kwitansi_col/ver_kwitansi_col_load.php
</commit_message>
<xml_diff>
--- a/RAPAT ANCOL/Meeting Coasta Villa Ancol.xlsx
+++ b/RAPAT ANCOL/Meeting Coasta Villa Ancol.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Jakarta 23 Oktober 2015</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Cases</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -150,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -258,11 +264,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -284,6 +299,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -385,12 +403,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A5:C22" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A5:C22"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A5:D22" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A5:D22"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="No" dataDxfId="2"/>
     <tableColumn id="2" name="Cases" dataDxfId="1"/>
     <tableColumn id="3" name="Keterangan" dataDxfId="0"/>
+    <tableColumn id="4" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -683,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C22"/>
+  <dimension ref="A2:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,19 +715,19 @@
     <col min="3" max="3" width="67.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="B2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
-    </row>
-    <row r="5" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="10"/>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -718,8 +737,11 @@
       <c r="C5" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>1</v>
       </c>
@@ -729,8 +751,11 @@
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -741,7 +766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>3</v>
       </c>
@@ -752,7 +777,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>4</v>
       </c>
@@ -762,8 +787,11 @@
       <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>5</v>
       </c>
@@ -773,8 +801,11 @@
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>6</v>
       </c>
@@ -785,7 +816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>7</v>
       </c>
@@ -796,7 +827,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>8</v>
       </c>
@@ -807,7 +838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>9</v>
       </c>
@@ -818,7 +849,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>10</v>
       </c>
@@ -829,7 +860,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>11</v>
       </c>
@@ -839,8 +870,11 @@
       <c r="C16" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>12</v>
       </c>
@@ -850,8 +884,11 @@
       <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>13</v>
       </c>
@@ -861,8 +898,11 @@
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>14</v>
       </c>
@@ -873,7 +913,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>15</v>
       </c>
@@ -884,7 +924,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>16</v>
       </c>
@@ -895,7 +935,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>

</xml_diff>

<commit_message>
MENU ROMBAK DATABASE ROMBAK DINAMIS TANDA TANGAN DI SPP ROMBAK SPP
</commit_message>
<xml_diff>
--- a/RAPAT ANCOL/Meeting Coasta Villa Ancol.xlsx
+++ b/RAPAT ANCOL/Meeting Coasta Villa Ancol.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>Jakarta 23 Oktober 2015</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Status sudah cetak. Notification. PAIJB:10% pembayaran. PPJB:20% pembayaran</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1242,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,7 +1307,9 @@
       <c r="C7" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="19">

</xml_diff>

<commit_message>
perbaikan bug di edit stok penjualan ketika update harga sk penambahan filed di agen dan koordinator/koordinator_load.php update Meeting Coasta Villa Ancol.xlsx
</commit_message>
<xml_diff>
--- a/RAPAT ANCOL/Meeting Coasta Villa Ancol.xlsx
+++ b/RAPAT ANCOL/Meeting Coasta Villa Ancol.xlsx
@@ -1,24 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UwAmp\www\market_ancol\RAPAT ANCOL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="7470" windowHeight="7470" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="7470" windowHeight="7470" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="23 Oktober 2015" sheetId="1" r:id="rId1"/>
-    <sheet name="5 November 2015" sheetId="2" r:id="rId2"/>
-    <sheet name="19 November 2015" sheetId="4" r:id="rId3"/>
-    <sheet name="25 November 2015" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="9 SEPTEMBER 2015" sheetId="6" r:id="rId1"/>
+    <sheet name="1 okt 2015" sheetId="7" r:id="rId2"/>
+    <sheet name="16 OKTOBER 2015" sheetId="8" r:id="rId3"/>
+    <sheet name="23 Oktober 2015" sheetId="1" r:id="rId4"/>
+    <sheet name="5 November 2015" sheetId="2" r:id="rId5"/>
+    <sheet name="19 November 2015" sheetId="4" r:id="rId6"/>
+    <sheet name="25 November 2015" sheetId="5" r:id="rId7"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="180">
   <si>
     <t>Jakarta 23 Oktober 2015</t>
   </si>
@@ -285,19 +293,299 @@
   </si>
   <si>
     <t>Sortir pilihan pembayaran pada jenis pembayaran dalam kwitansi</t>
+  </si>
+  <si>
+    <t>NEXT CONTRACT</t>
+  </si>
+  <si>
+    <t>NO KUITANSI BISA BERBEDA DENGAN ORLANSOFT</t>
+  </si>
+  <si>
+    <t>OTORISASI USER</t>
+  </si>
+  <si>
+    <t>INPUT MANUAL PEMBAYARAN VIA REKENING KORAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   FORMAT : CEKLIS PEMBAYARAN, </t>
+  </si>
+  <si>
+    <t>GRACE PERIODE : 14 HARI SETELAH TANGGAL JATUH TEMPO</t>
+  </si>
+  <si>
+    <t>LAPORAN COLLECTION : KPR, CICILAN BERTAHAP, CASH KERAS</t>
+  </si>
+  <si>
+    <t>DIBIKIN SUB NYA</t>
+  </si>
+  <si>
+    <t>FORMAT SURAT JATUH TEMPO</t>
+  </si>
+  <si>
+    <t>FORMAT NO VA: 888LANTAIUNIT</t>
+  </si>
+  <si>
+    <t>KUITANSI ADA CEKLIS DARI USER (PEJABAT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    STAF -&gt; SUPERVISOR -&gt; MANAGER (SUDAH)</t>
+  </si>
+  <si>
+    <t>USER : STAF, SUPERVISOR , MANAGER</t>
+  </si>
+  <si>
+    <t>PPJB -&gt; PAIJB (uda)</t>
+  </si>
+  <si>
+    <t>KARTU KUNING DI COLLECTION ( Sudah ada)</t>
+  </si>
+  <si>
+    <t>01686 (KODE PERUSAHAAN) (uda)</t>
+  </si>
+  <si>
+    <t>FORMAT UPLOAD KE SISTEM ORLANSOFT VIA EXCEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KUITANSI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ada pilihan berupa ceklis via edc , giro/cek, bank O, virtual account </t>
+  </si>
+  <si>
+    <t>FORMAT PPJB</t>
+  </si>
+  <si>
+    <t>DAFTAR TAGIHAN BANK</t>
+  </si>
+  <si>
+    <t>Muncul Hanya bank BCA Saja</t>
+  </si>
+  <si>
+    <t>penentuan format VA</t>
+  </si>
+  <si>
+    <t>Jakarta 9 SEPTEMBER 2015</t>
+  </si>
+  <si>
+    <t>NOTULENSI RAPAT ANCOL</t>
+  </si>
+  <si>
+    <t>TANGGAL 1 OKTOBER 2015</t>
+  </si>
+  <si>
+    <t>KETERANGAN</t>
+  </si>
+  <si>
+    <t>DAFTAR PPJB</t>
+  </si>
+  <si>
+    <t>SUDAH</t>
+  </si>
+  <si>
+    <t>LUAS BANGUNAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KELURAHAN , KECAMATAN </t>
+  </si>
+  <si>
+    <t>FORMAT SP</t>
+  </si>
+  <si>
+    <t>BATASAN OTORITAS</t>
+  </si>
+  <si>
+    <t>BELUM</t>
+  </si>
+  <si>
+    <t>KEUANGAN : COLLECTION</t>
+  </si>
+  <si>
+    <t>MARKETING : PPJB, SP</t>
+  </si>
+  <si>
+    <t>KODE VA:</t>
+  </si>
+  <si>
+    <t>KONDO : 888</t>
+  </si>
+  <si>
+    <t>PODIUM : 889, LANTAI : 00, UNIT : 1 - 30</t>
+  </si>
+  <si>
+    <t>FORMAT SURAT JATUH TEMPO, SOMASI 1, SOMASI 2, SOMASI</t>
+  </si>
+  <si>
+    <t>BELUM ADA FORMAT</t>
+  </si>
+  <si>
+    <t>KETENTUAN JATUH TEMPO:</t>
+  </si>
+  <si>
+    <t>CEK</t>
+  </si>
+  <si>
+    <t>MASTER STOK UPDATE EXCEL</t>
+  </si>
+  <si>
+    <t>LAPORAN KE ORLANSOFT : RENCANA PENERIMAAN DAN REALISASI  (samain kayak AA Master Condo)</t>
+  </si>
+  <si>
+    <t>LAYOUT SOLD</t>
+  </si>
+  <si>
+    <t>RUMUS PERHITUNGAN DENDA</t>
+  </si>
+  <si>
+    <t>sudah</t>
+  </si>
+  <si>
+    <t>PRICELIST DI EXCEL</t>
+  </si>
+  <si>
+    <t>MODUL</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>BOOKING FEE</t>
+  </si>
+  <si>
+    <t>2000000 ATAU ISI MANUAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANGGAL RENCANA </t>
+  </si>
+  <si>
+    <t>14 HARI KERJA SETELAH BOOKING FEE</t>
+  </si>
+  <si>
+    <t>ATAU TENTUKAN TANGGAL</t>
+  </si>
+  <si>
+    <t>RENCANA</t>
+  </si>
+  <si>
+    <t>NILAI BOOKING FEE MASUK KE SP</t>
+  </si>
+  <si>
+    <t>MUNCUL DI ANGSURAN 1</t>
+  </si>
+  <si>
+    <t>MENGURANGI ANGSURAN 1</t>
+  </si>
+  <si>
+    <t>PENGISIAN TTS</t>
+  </si>
+  <si>
+    <t>OTOMATIS DICARI DAN DIISI DENGAN KODE BLOK YANG TERJUAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TANDA TERIMA DAN KUITANSI </t>
+  </si>
+  <si>
+    <t>TIDAK ADA TANDA TANGAN PEMBELI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORMAT PIUTANG SAMAIN AR </t>
+  </si>
+  <si>
+    <t>LIHAT EXCEL AR CONDO TAB AR</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>DIILANGIN PT GRAHA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP </t>
+  </si>
+  <si>
+    <t>TAMBAHIN SALES, GM PROPERTI 1, GM SALES</t>
+  </si>
+  <si>
+    <t>ALAMAT NPWP</t>
+  </si>
+  <si>
+    <t>DIHAPUS</t>
+  </si>
+  <si>
+    <t>ALAMAT RUMAH</t>
+  </si>
+  <si>
+    <t>CEKLIS -&gt; NGISI ALAMAT KORESPODENSI</t>
+  </si>
+  <si>
+    <t>SALES, GM PROPERTI 1, GM SALES</t>
+  </si>
+  <si>
+    <t>ENTRI MANUAL</t>
+  </si>
+  <si>
+    <t>JIKA CB36X</t>
+  </si>
+  <si>
+    <t>BALOON PAYMENT : PAKE RUMUS 5% UTK 1O BULAN, 15% UTK 12 BLN, 10% UTK 14 BLN, 70% SISANYA</t>
+  </si>
+  <si>
+    <t>INPUTAN OTOMATIS CAPSLOK</t>
+  </si>
+  <si>
+    <t>POSISI UNIT TERJUAL</t>
+  </si>
+  <si>
+    <t>DIPAKE BUTTON UNTUK REFRESH</t>
+  </si>
+  <si>
+    <t>FORM PENJUALAN</t>
+  </si>
+  <si>
+    <t>BGB, REFERAL, MEMBER</t>
+  </si>
+  <si>
+    <t>DAFTAR SPP</t>
+  </si>
+  <si>
+    <t>MASIH ADA LUAS TANAH</t>
+  </si>
+  <si>
+    <t>PPJB</t>
+  </si>
+  <si>
+    <t>TOTAL HARGA BELUM TO MONEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KUITANSI PENJUALAN </t>
+  </si>
+  <si>
+    <t>POP UP DILEBARIN</t>
+  </si>
+  <si>
+    <t>CETAK KARTU PEMBELI</t>
+  </si>
+  <si>
+    <t>POP UP EROR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -315,8 +603,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,8 +633,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -485,12 +795,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -518,84 +885,204 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="38">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -686,13 +1173,6 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -704,6 +1184,13 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -808,13 +1295,6 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -826,6 +1306,13 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1047,17 +1534,20 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A5:D22" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
-  <autoFilter ref="A5:D22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A5:D24" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+  <autoFilter ref="A5:D24"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="No" dataDxfId="26"/>
-    <tableColumn id="2" name="Cases" dataDxfId="25"/>
-    <tableColumn id="3" name="Keterangan" dataDxfId="24"/>
+    <tableColumn id="1" name="No" dataDxfId="1"/>
+    <tableColumn id="2" name="Cases" dataDxfId="0"/>
+    <tableColumn id="3" name="Keterangan" dataDxfId="2"/>
     <tableColumn id="4" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1065,39 +1555,64 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table17" displayName="Table17" ref="A2:C24" totalsRowShown="0">
+  <autoFilter ref="A2:C24"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="MODUL"/>
+    <tableColumn id="2" name="KETERANGAN"/>
+    <tableColumn id="3" name="status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A5:D22" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="A5:D22"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="No" dataDxfId="33"/>
+    <tableColumn id="2" name="Cases" dataDxfId="32"/>
+    <tableColumn id="3" name="Keterangan" dataDxfId="31"/>
+    <tableColumn id="4" name="Status"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27">
   <autoFilter ref="A4:D5"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="No" dataDxfId="19"/>
-    <tableColumn id="2" name="Cases" dataDxfId="18"/>
-    <tableColumn id="3" name="Keterangan" dataDxfId="17"/>
-    <tableColumn id="4" name="Status" dataDxfId="16"/>
+    <tableColumn id="1" name="No" dataDxfId="26"/>
+    <tableColumn id="2" name="Cases" dataDxfId="25"/>
+    <tableColumn id="3" name="Keterangan" dataDxfId="24"/>
+    <tableColumn id="4" name="Status" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
   <autoFilter ref="A4:D5"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="No" dataDxfId="11"/>
-    <tableColumn id="2" name="Cases" dataDxfId="10"/>
-    <tableColumn id="3" name="Keterangan" dataDxfId="9"/>
-    <tableColumn id="4" name="Status" dataDxfId="8"/>
+    <tableColumn id="1" name="No" dataDxfId="18"/>
+    <tableColumn id="2" name="Cases" dataDxfId="17"/>
+    <tableColumn id="3" name="Keterangan" dataDxfId="16"/>
+    <tableColumn id="4" name="Status" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
   <autoFilter ref="A4:D5"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="No" dataDxfId="3"/>
-    <tableColumn id="2" name="Cases" dataDxfId="2"/>
-    <tableColumn id="3" name="Keterangan" dataDxfId="1"/>
-    <tableColumn id="4" name="Status" dataDxfId="0"/>
+    <tableColumn id="1" name="No" dataDxfId="10"/>
+    <tableColumn id="2" name="Cases" dataDxfId="9"/>
+    <tableColumn id="3" name="Keterangan" dataDxfId="8"/>
+    <tableColumn id="4" name="Status" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1146,7 +1661,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1181,7 +1696,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1390,31 +1905,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D22"/>
+  <dimension ref="A2:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57" customWidth="1"/>
     <col min="3" max="3" width="67.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="26"/>
+      <c r="A2" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="38"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="38"/>
     </row>
     <row r="5" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1431,11 +1946,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="39">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
@@ -1444,190 +1959,221 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="39">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="39">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="39">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>3</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="4"/>
       <c r="D9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="39">
         <v>5</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="B10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="4"/>
       <c r="D10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="39"/>
+      <c r="B11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="39">
         <v>6</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="39">
         <v>7</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>7</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="B13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="39">
         <v>8</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="B14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="39"/>
+      <c r="B15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="39">
         <v>9</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>10</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>11</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="B16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="4"/>
       <c r="D16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>12</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>9</v>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="39">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
-        <v>13</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>24</v>
+      <c r="A18" s="39">
+        <v>11</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="D18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="39">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="39"/>
+      <c r="B20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="39">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="39">
         <v>14</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="B22" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="39">
         <v>15</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="B23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="39">
         <v>16</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
+      <c r="B24" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1643,10 +2189,810 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.42578125" style="42" customWidth="1"/>
+    <col min="2" max="2" width="98.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+    </row>
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="43">
+        <v>1</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="43">
+        <v>2</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="43">
+        <v>3</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="45" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="43">
+        <v>4</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="43">
+        <v>5</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="43"/>
+      <c r="B11" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="43"/>
+      <c r="B12" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="43"/>
+      <c r="B13" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="43"/>
+      <c r="B14" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="43"/>
+      <c r="B15" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="45" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="43"/>
+      <c r="B16" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="43"/>
+      <c r="B17" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" s="45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="43"/>
+      <c r="B18" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" s="45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="43"/>
+      <c r="B19" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="43"/>
+      <c r="B20" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="43"/>
+      <c r="B21" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="43"/>
+      <c r="B22" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="43"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="44"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="43"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="44"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="43"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="44"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="44"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="44"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="44"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>175</v>
+      </c>
+      <c r="C22" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="38"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="38"/>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>9</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>11</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>13</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>14</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>15</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>16</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,16 +3004,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="38"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="38"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -1699,7 +3045,9 @@
       <c r="C6" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
@@ -1725,7 +3073,9 @@
       <c r="C8" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="20"/>
+      <c r="D8" s="20" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
@@ -1737,7 +3087,9 @@
       <c r="C9" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="20"/>
+      <c r="D9" s="20" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
@@ -1755,7 +3107,9 @@
       <c r="C11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="25">
@@ -1767,7 +3121,9 @@
       <c r="C12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="25">
@@ -1779,7 +3135,9 @@
       <c r="C13" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="25">
@@ -1791,7 +3149,9 @@
       <c r="C14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="25">
@@ -1803,7 +3163,9 @@
       <c r="C15" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
@@ -1824,7 +3186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -1841,16 +3203,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="38"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="38"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -1901,58 +3263,58 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="28"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="37"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="36"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="31"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="30"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="34"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="33"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="34"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="33"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="34"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="33"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="34"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="33"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="34"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="33"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="34"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1967,12 +3329,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1980,20 +3342,20 @@
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="67.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="38"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="38"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -2025,7 +3387,9 @@
       <c r="C6" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
@@ -2037,103 +3401,109 @@
       <c r="C7" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
+      <c r="A8" s="26">
         <v>3</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="28"/>
+      <c r="D8" s="27" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="27">
+      <c r="A9" s="26">
         <v>4</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="28"/>
+      <c r="D9" s="27"/>
     </row>
     <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="27">
+      <c r="A10" s="26">
         <v>5</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="28"/>
+      <c r="D10" s="27"/>
     </row>
     <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="27">
+      <c r="A11" s="26">
         <v>6</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="28"/>
+      <c r="D11" s="27"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
+      <c r="A12" s="26">
         <v>7</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="27">
+      <c r="A13" s="26">
         <v>8</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="28"/>
+      <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="27">
+      <c r="A14" s="26">
         <v>9</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="28"/>
+      <c r="D14" s="27"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="27">
+      <c r="A15" s="26">
         <v>10</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="27" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
@@ -2196,7 +3566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
update home update kwitansi
</commit_message>
<xml_diff>
--- a/RAPAT ANCOL/Meeting Coasta Villa Ancol.xlsx
+++ b/RAPAT ANCOL/Meeting Coasta Villa Ancol.xlsx
@@ -21,12 +21,12 @@
     <sheet name="25 November 2015" sheetId="5" r:id="rId7"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="180">
   <si>
     <t>Jakarta 23 Oktober 2015</t>
   </si>
@@ -954,16 +954,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -990,6 +984,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -998,91 +998,6 @@
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="38">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1528,6 +1443,91 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1542,12 +1542,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A5:D24" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A5:D24" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="A5:D24"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="No" dataDxfId="1"/>
-    <tableColumn id="2" name="Cases" dataDxfId="0"/>
-    <tableColumn id="3" name="Keterangan" dataDxfId="2"/>
+    <tableColumn id="1" name="No" dataDxfId="33"/>
+    <tableColumn id="2" name="Cases" dataDxfId="32"/>
+    <tableColumn id="3" name="Keterangan" dataDxfId="31"/>
     <tableColumn id="4" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1567,12 +1567,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A5:D22" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A5:D22" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="A5:D22"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="No" dataDxfId="33"/>
-    <tableColumn id="2" name="Cases" dataDxfId="32"/>
-    <tableColumn id="3" name="Keterangan" dataDxfId="31"/>
+    <tableColumn id="1" name="No" dataDxfId="26"/>
+    <tableColumn id="2" name="Cases" dataDxfId="25"/>
+    <tableColumn id="3" name="Keterangan" dataDxfId="24"/>
     <tableColumn id="4" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1580,39 +1580,39 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
   <autoFilter ref="A4:D5"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="No" dataDxfId="26"/>
-    <tableColumn id="2" name="Cases" dataDxfId="25"/>
-    <tableColumn id="3" name="Keterangan" dataDxfId="24"/>
-    <tableColumn id="4" name="Status" dataDxfId="23"/>
+    <tableColumn id="1" name="No" dataDxfId="19"/>
+    <tableColumn id="2" name="Cases" dataDxfId="18"/>
+    <tableColumn id="3" name="Keterangan" dataDxfId="17"/>
+    <tableColumn id="4" name="Status" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
   <autoFilter ref="A4:D5"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="No" dataDxfId="18"/>
-    <tableColumn id="2" name="Cases" dataDxfId="17"/>
-    <tableColumn id="3" name="Keterangan" dataDxfId="16"/>
-    <tableColumn id="4" name="Status" dataDxfId="15"/>
+    <tableColumn id="1" name="No" dataDxfId="11"/>
+    <tableColumn id="2" name="Cases" dataDxfId="10"/>
+    <tableColumn id="3" name="Keterangan" dataDxfId="9"/>
+    <tableColumn id="4" name="Status" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
   <autoFilter ref="A4:D5"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="No" dataDxfId="10"/>
-    <tableColumn id="2" name="Cases" dataDxfId="9"/>
-    <tableColumn id="3" name="Keterangan" dataDxfId="8"/>
-    <tableColumn id="4" name="Status" dataDxfId="7"/>
+    <tableColumn id="1" name="No" dataDxfId="3"/>
+    <tableColumn id="2" name="Cases" dataDxfId="2"/>
+    <tableColumn id="3" name="Keterangan" dataDxfId="1"/>
+    <tableColumn id="4" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1920,16 +1920,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="51"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="51"/>
     </row>
     <row r="5" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1946,7 +1946,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="39">
+      <c r="A6" s="38">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1960,7 +1960,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="39">
+      <c r="A7" s="38">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1974,7 +1974,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="39">
+      <c r="A8" s="38">
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1986,7 +1986,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="39">
+      <c r="A9" s="38">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1998,7 +1998,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="39">
+      <c r="A10" s="38">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2010,7 +2010,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="1" t="s">
         <v>93</v>
       </c>
@@ -2020,7 +2020,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="39">
+      <c r="A12" s="38">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2032,7 +2032,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="39">
+      <c r="A13" s="38">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2044,7 +2044,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="39">
+      <c r="A14" s="38">
         <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2056,7 +2056,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="1" t="s">
         <v>96</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="39">
+      <c r="A16" s="38">
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2078,7 +2078,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="39">
+      <c r="A17" s="38">
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -2092,7 +2092,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="39">
+      <c r="A18" s="38">
         <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -2106,7 +2106,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="39">
+      <c r="A19" s="38">
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2118,7 +2118,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
+      <c r="A20" s="38"/>
       <c r="B20" s="1" t="s">
         <v>100</v>
       </c>
@@ -2128,7 +2128,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="39">
+      <c r="A21" s="38">
         <v>13</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2140,7 +2140,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="39">
+      <c r="A22" s="38">
         <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2152,7 +2152,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="39">
+      <c r="A23" s="38">
         <v>15</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2164,10 +2164,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="39">
+      <c r="A24" s="38">
         <v>16</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="39" t="s">
         <v>104</v>
       </c>
       <c r="C24" s="2"/>
@@ -2197,235 +2197,235 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="42" customWidth="1"/>
-    <col min="2" max="2" width="98.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="47" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="42"/>
+    <col min="1" max="1" width="8.42578125" style="40" customWidth="1"/>
+    <col min="2" max="2" width="98.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
     </row>
     <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="50" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="43">
+      <c r="A6" s="41">
         <v>1</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="43" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="43">
+      <c r="A7" s="41">
         <v>2</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="43" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="43">
+      <c r="A8" s="41">
         <v>3</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="43" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="43">
+      <c r="A9" s="41">
         <v>4</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="43" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="43">
+      <c r="A10" s="41">
         <v>5</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="43" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="44" t="s">
+      <c r="A11" s="41"/>
+      <c r="B11" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="43" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="44" t="s">
+      <c r="A12" s="41"/>
+      <c r="B12" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="43" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="44" t="s">
+      <c r="A13" s="41"/>
+      <c r="B13" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="43" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
-      <c r="B14" s="44" t="s">
+      <c r="A14" s="41"/>
+      <c r="B14" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="43" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="44" t="s">
+      <c r="A15" s="41"/>
+      <c r="B15" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="43" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="44" t="s">
+      <c r="A16" s="41"/>
+      <c r="B16" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="43" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="44" t="s">
+      <c r="A17" s="41"/>
+      <c r="B17" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="D17" s="45" t="s">
+      <c r="D17" s="43" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="44" t="s">
+      <c r="A18" s="41"/>
+      <c r="B18" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="D18" s="45" t="s">
+      <c r="D18" s="43" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="44" t="s">
+      <c r="A19" s="41"/>
+      <c r="B19" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="D19" s="45" t="s">
+      <c r="D19" s="43" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="44" t="s">
+      <c r="A20" s="41"/>
+      <c r="B20" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="D20" s="45" t="s">
+      <c r="D20" s="43" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="44" t="s">
+      <c r="A21" s="41"/>
+      <c r="B21" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D21" s="43" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="44" t="s">
+      <c r="A22" s="41"/>
+      <c r="B22" s="42" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="45" t="s">
+      <c r="D22" s="43" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="44"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="42"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="46"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="44"/>
+      <c r="A24" s="41"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="42"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="43"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="44"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="42"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="44"/>
-      <c r="B26" s="44"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="44"/>
+      <c r="A26" s="42"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="42"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="44"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2447,252 +2447,252 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="42"/>
+    <col min="1" max="1" width="30.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="40" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="40" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="40" t="s">
         <v>171</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="40" t="s">
         <v>177</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="40" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="40" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2721,16 +2721,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="51"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="38"/>
+      <c r="B3" s="51"/>
     </row>
     <row r="5" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -3004,16 +3004,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="51"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -3203,16 +3203,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="51"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -3333,8 +3333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3346,16 +3346,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="38"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="51"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -3429,7 +3429,9 @@
       <c r="C9" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="27"/>
+      <c r="D9" s="27" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
@@ -3441,7 +3443,9 @@
       <c r="C10" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="27"/>
+      <c r="D10" s="27" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="26">
@@ -3515,7 +3519,9 @@
       <c r="C16" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="20" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="19">

</xml_diff>

<commit_message>
Update size column login id jadi 30 dan default database di index.php
</commit_message>
<xml_diff>
--- a/RAPAT ANCOL/Meeting Coasta Villa Ancol.xlsx
+++ b/RAPAT ANCOL/Meeting Coasta Villa Ancol.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UwAmp\www\market_ancol\RAPAT ANCOL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="7470" windowHeight="7470" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="180" windowWidth="7470" windowHeight="7410" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="9 SEPTEMBER 2015" sheetId="6" r:id="rId1"/>
@@ -19,14 +14,15 @@
     <sheet name="5 November 2015" sheetId="2" r:id="rId5"/>
     <sheet name="19 November 2015" sheetId="4" r:id="rId6"/>
     <sheet name="25 November 2015" sheetId="5" r:id="rId7"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId8"/>
+    <sheet name="8 Desember 2015" sheetId="10" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="183">
   <si>
     <t>Jakarta 23 Oktober 2015</t>
   </si>
@@ -566,12 +562,21 @@
   </si>
   <si>
     <t>POP UP EROR</t>
+  </si>
+  <si>
+    <t>Jakarta 8 Desember 2015</t>
+  </si>
+  <si>
+    <t>Modul Orlansoft</t>
+  </si>
+  <si>
+    <t>Sinkronisasi data untuk orlansoft ke dalam tabel temporari sybase central</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -997,7 +1002,7 @@
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="46">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1327,6 +1332,128 @@
     <dxf>
       <border outline="0">
         <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
@@ -1542,12 +1669,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A5:D24" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A5:D24" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43" totalsRowBorderDxfId="42">
   <autoFilter ref="A5:D24"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="No" dataDxfId="33"/>
-    <tableColumn id="2" name="Cases" dataDxfId="32"/>
-    <tableColumn id="3" name="Keterangan" dataDxfId="31"/>
+    <tableColumn id="1" name="No" dataDxfId="41"/>
+    <tableColumn id="2" name="Cases" dataDxfId="40"/>
+    <tableColumn id="3" name="Keterangan" dataDxfId="39"/>
     <tableColumn id="4" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1567,12 +1694,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A5:D22" totalsRowShown="0" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A5:D22" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="A5:D22"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="No" dataDxfId="26"/>
-    <tableColumn id="2" name="Cases" dataDxfId="25"/>
-    <tableColumn id="3" name="Keterangan" dataDxfId="24"/>
+    <tableColumn id="1" name="No" dataDxfId="34"/>
+    <tableColumn id="2" name="Cases" dataDxfId="33"/>
+    <tableColumn id="3" name="Keterangan" dataDxfId="32"/>
     <tableColumn id="4" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1580,7 +1707,20 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28">
+  <autoFilter ref="A4:D5"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="No" dataDxfId="27"/>
+    <tableColumn id="2" name="Cases" dataDxfId="26"/>
+    <tableColumn id="3" name="Keterangan" dataDxfId="25"/>
+    <tableColumn id="4" name="Status" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
   <autoFilter ref="A4:D5"/>
   <tableColumns count="4">
     <tableColumn id="1" name="No" dataDxfId="19"/>
@@ -1592,8 +1732,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
   <autoFilter ref="A4:D5"/>
   <tableColumns count="4">
     <tableColumn id="1" name="No" dataDxfId="11"/>
@@ -1605,8 +1745,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table1458" displayName="Table1458" ref="A4:D5" insertRow="1" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
   <autoFilter ref="A4:D5"/>
   <tableColumns count="4">
     <tableColumn id="1" name="No" dataDxfId="3"/>
@@ -1661,7 +1801,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1696,7 +1836,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3333,7 +3473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -3576,6 +3716,183 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="67.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="51"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="51"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+    </row>
+    <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
+        <v>1</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="19">
+        <v>2</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
+        <v>3</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="27"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="26">
+        <v>4</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="27"/>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="26">
+        <v>5</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="27"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="26">
+        <v>6</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="27"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="26">
+        <v>7</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="27"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
+        <v>8</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="27"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="26">
+        <v>9</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="27"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
+        <v>10</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="27"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="19">
+        <v>11</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="19">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="19">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="19">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>